<commit_message>
tmp add setting page
</commit_message>
<xml_diff>
--- a/src/assets/docs/Import_Khach_Hang.xlsx
+++ b/src/assets/docs/Import_Khach_Hang.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="166">
   <si>
     <t>VÕ VĂN HÙNG</t>
   </si>
@@ -494,6 +494,33 @@
   </si>
   <si>
     <t>Thay nhớt</t>
+  </si>
+  <si>
+    <t>SIRIUS</t>
+  </si>
+  <si>
+    <t>JUPITER</t>
+  </si>
+  <si>
+    <t>EXCITER</t>
+  </si>
+  <si>
+    <t>FREE GO</t>
+  </si>
+  <si>
+    <t>NOZZA GRANDE</t>
+  </si>
+  <si>
+    <t>ACRUZO</t>
+  </si>
+  <si>
+    <t>JANUS</t>
+  </si>
+  <si>
+    <t>NVX 125</t>
+  </si>
+  <si>
+    <t>XE KHÁC</t>
   </si>
 </sst>
 </file>
@@ -929,9 +956,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O113"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1067,7 +1092,7 @@
         <v>123</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>102</v>
+        <v>80</v>
       </c>
       <c r="I3" s="10" t="s">
         <v>62</v>
@@ -1108,7 +1133,7 @@
         <v>129</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>106</v>
+        <v>80</v>
       </c>
       <c r="I4" s="10" t="s">
         <v>63</v>
@@ -1153,7 +1178,7 @@
         <v>125</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>119</v>
+        <v>80</v>
       </c>
       <c r="I5" s="10" t="s">
         <v>64</v>
@@ -1196,7 +1221,7 @@
         <v>125</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>117</v>
+        <v>80</v>
       </c>
       <c r="I6" s="10" t="s">
         <v>65</v>
@@ -1237,7 +1262,7 @@
         <v>125</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>108</v>
+        <v>80</v>
       </c>
       <c r="I7" s="10" t="s">
         <v>66</v>
@@ -1280,7 +1305,7 @@
         <v>125</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>107</v>
+        <v>80</v>
       </c>
       <c r="I8" s="10" t="s">
         <v>152</v>
@@ -1327,7 +1352,7 @@
         <v>126</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>93</v>
+        <v>157</v>
       </c>
       <c r="I9" s="10" t="s">
         <v>152</v>
@@ -1369,7 +1394,9 @@
       <c r="G10" s="8" t="s">
         <v>123</v>
       </c>
-      <c r="H10" s="7"/>
+      <c r="H10" s="7" t="s">
+        <v>159</v>
+      </c>
       <c r="I10" s="10" t="s">
         <v>67</v>
       </c>
@@ -1411,7 +1438,7 @@
         <v>129</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>94</v>
+        <v>160</v>
       </c>
       <c r="I11" s="10"/>
       <c r="J11" s="8" t="s">
@@ -1452,7 +1479,7 @@
         <v>125</v>
       </c>
       <c r="H12" s="7" t="s">
-        <v>114</v>
+        <v>161</v>
       </c>
       <c r="I12" s="10" t="s">
         <v>68</v>
@@ -1493,7 +1520,7 @@
         <v>127</v>
       </c>
       <c r="H13" s="7" t="s">
-        <v>78</v>
+        <v>162</v>
       </c>
       <c r="I13" s="10" t="s">
         <v>69</v>
@@ -1534,7 +1561,7 @@
         <v>128</v>
       </c>
       <c r="H14" s="7" t="s">
-        <v>79</v>
+        <v>163</v>
       </c>
       <c r="I14" s="10" t="s">
         <v>70</v>
@@ -1577,7 +1604,7 @@
         <v>122</v>
       </c>
       <c r="H15" s="7" t="s">
-        <v>80</v>
+        <v>164</v>
       </c>
       <c r="I15" s="10" t="s">
         <v>71</v>
@@ -1620,7 +1647,7 @@
         <v>124</v>
       </c>
       <c r="H16" s="7" t="s">
-        <v>81</v>
+        <v>165</v>
       </c>
       <c r="I16" s="10" t="s">
         <v>72</v>
@@ -3292,7 +3319,7 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="6">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="7">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Sheet1!$A$2:$A$9</xm:f>
@@ -3303,7 +3330,7 @@
           <x14:formula1>
             <xm:f>Sheet1!$C$2:$C$43</xm:f>
           </x14:formula1>
-          <xm:sqref>H2:H113</xm:sqref>
+          <xm:sqref>H17:H113</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
@@ -3329,6 +3356,12 @@
           </x14:formula1>
           <xm:sqref>M2:M16</xm:sqref>
         </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Sheet1!$C$2:$C$52</xm:f>
+          </x14:formula1>
+          <xm:sqref>H2:H16</xm:sqref>
+        </x14:dataValidation>
       </x14:dataValidations>
     </ext>
   </extLst>
@@ -3337,7 +3370,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J43"/>
+  <dimension ref="A1:J52"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3651,6 +3684,51 @@
         <v>119</v>
       </c>
     </row>
+    <row r="44" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C44" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="45" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C45" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="46" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C46" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="47" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C47" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="48" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C48" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="49" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C49" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="50" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C50" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="51" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C51" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="52" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C52" t="s">
+        <v>165</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>